<commit_message>
Gráficas de transmitancia y absorbancia
</commit_message>
<xml_diff>
--- a/mediciones.xlsx
+++ b/mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP desktop\Documents\Trimestre19P\ILC\Instrumentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D55A73-685B-459D-B732-294CFA7EE286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC56F19-5E8F-4E51-87CB-441EBD259A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{13AECB73-DCFA-4E9C-88B0-B89AB381D81E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Longitud de onda</t>
   </si>
@@ -39,13 +39,22 @@
     <t>Voltaje (V)</t>
   </si>
   <si>
-    <t>Tansmitancia (T)</t>
+    <t>Absorbancia (A)</t>
+  </si>
+  <si>
+    <t>Transmitancia (T)</t>
+  </si>
+  <si>
+    <t>Tansmitancia (T%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,13 +84,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -98,6 +113,2007 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Transmitancia</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="110"/>
+                <c:pt idx="0">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>535</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>665</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>685</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>695</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>755</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>765</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>795</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>805</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>815</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>835</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>845</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>855</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>865</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>880</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$2:$D$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="110"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6631-48C6-81CC-02109A8E15A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Absorbancia</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$E$2:$E$111</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="110"/>
+                <c:pt idx="0">
+                  <c:v>0.63095734448019325</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69183097091893653</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69183097091893653</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.660693448007596</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60255958607435778</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48977881936844614</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38904514499428056</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.30199517204020154</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2630267991895382</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22908676527677729</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15848931924611132</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.19498445997580449</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.17782794100389224</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17378008287493749</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.16595869074375599</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.16595869074375599</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16982436524617442</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.18620871366628672</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.20892961308540392</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.25118864315095801</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.28840315031266056</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.30902954325135895</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.31622776601683794</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.30902954325135895</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.30199517204020154</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.30199517204020154</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.31622776601683794</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.32359365692962827</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.31622776601683794</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.29512092266663847</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.25703957827688634</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.22908676527677729</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.22908676527677729</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.23988329190194901</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.27542287033381663</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.30902954325135895</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.34673685045253166</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.3981071705534972</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.41686938347033536</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.38904514499428056</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.33113112148259105</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.28183829312644532</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.21877616239495523</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.19498445997580449</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.19952623149688795</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.22908676527677729</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.31622776601683794</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47863009232263831</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.61659500186148219</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.75857757502918366</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.81283051616409918</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.81283051616409918</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.74131024130091738</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.60255958607435778</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.47863009232263831</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.38018939632056115</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.28840315031266056</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.23442288153199217</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.20417379446695291</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.19498445997580449</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.19054607179632471</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.19498445997580449</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.19498445997580449</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.19952623149688795</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.21379620895022314</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.22908676527677729</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.23988329190194901</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.2630267991895382</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.28840315031266056</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.32359365692962827</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.36307805477010135</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.37153522909717251</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.3981071705534972</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.41686938347033536</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.44668359215096315</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.44668359215096315</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.45708818961487502</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.44668359215096315</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.40738027780411268</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.38904514499428056</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.34673685045253166</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.32359365692962827</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.30902954325135895</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.28840315031266056</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.2630267991895382</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.25118864315095801</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.23988329190194901</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.22908676527677729</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.21379620895022314</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.21379620895022314</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.20417379446695291</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.20417379446695291</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.19952623149688795</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.19498445997580449</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.19054607179632471</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.18620871366628672</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.18197008586099833</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.18197008586099833</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.17782794100389224</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.17782794100389224</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.17782794100389224</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.18197008586099833</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.19054607179632471</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.20417379446695291</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.22908676527677729</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.25703957827688634</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.28840315031266056</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.31622776601683794</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.33113112148259105</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.34673685045253166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{000000F7-6631-48C6-81CC-02109A8E15A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="398089800"/>
+        <c:axId val="398090128"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="398089800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Longitud</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> de onda (nm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398090128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="398090128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Transmitancia</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398089800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6901815A-121B-4A55-8A68-2CE355851DC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,19 +2413,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CB8A4A-17EF-4774-BF88-5033E5449A90}">
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="3" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -417,10 +2433,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>335</v>
       </c>
@@ -430,8 +2452,16 @@
       <c r="C2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>C2/100</f>
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="4">
+        <f>10^(-C2/100)</f>
+        <v>0.63095734448019325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+5</f>
         <v>340</v>
@@ -442,10 +2472,18 @@
       <c r="C3">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3/100</f>
+        <v>0.16</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E66" si="1">10^(-C3/100)</f>
+        <v>0.69183097091893653</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A37" si="0">A3+5</f>
+        <f t="shared" ref="A4:A37" si="2">A3+5</f>
         <v>345</v>
       </c>
       <c r="B4">
@@ -454,10 +2492,18 @@
       <c r="C4">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.69183097091893653</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>350</v>
       </c>
       <c r="B5">
@@ -466,10 +2512,18 @@
       <c r="C5">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.660693448007596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>355</v>
       </c>
       <c r="B6">
@@ -478,10 +2532,18 @@
       <c r="C6">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.60255958607435778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>360</v>
       </c>
       <c r="B7">
@@ -490,10 +2552,18 @@
       <c r="C7">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.31</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.48977881936844614</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>365</v>
       </c>
       <c r="B8">
@@ -502,10 +2572,18 @@
       <c r="C8">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.41</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.38904514499428056</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>370</v>
       </c>
       <c r="B9">
@@ -514,10 +2592,18 @@
       <c r="C9">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30199517204020154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>375</v>
       </c>
       <c r="B10">
@@ -526,10 +2612,18 @@
       <c r="C10">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.2630267991895382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>380</v>
       </c>
       <c r="B11">
@@ -538,10 +2632,18 @@
       <c r="C11">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.22908676527677729</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>385</v>
       </c>
       <c r="B12">
@@ -550,10 +2652,18 @@
       <c r="C12">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.15848931924611132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>390</v>
       </c>
       <c r="B13">
@@ -562,10 +2672,18 @@
       <c r="C13">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19498445997580449</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>395</v>
       </c>
       <c r="B14">
@@ -574,10 +2692,18 @@
       <c r="C14">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.17782794100389224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="B15">
@@ -586,10 +2712,18 @@
       <c r="C15">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.76</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="1"/>
+        <v>0.17378008287493749</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>405</v>
       </c>
       <c r="B16">
@@ -598,10 +2732,18 @@
       <c r="C16">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16595869074375599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>410</v>
       </c>
       <c r="B17">
@@ -610,10 +2752,18 @@
       <c r="C17">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16595869074375599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>415</v>
       </c>
       <c r="B18">
@@ -622,10 +2772,18 @@
       <c r="C18">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.77</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16982436524617442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>420</v>
       </c>
       <c r="B19">
@@ -634,10 +2792,18 @@
       <c r="C19">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0.73</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="1"/>
+        <v>0.18620871366628672</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>425</v>
       </c>
       <c r="B20">
@@ -646,10 +2812,18 @@
       <c r="C20">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0.68</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="1"/>
+        <v>0.20892961308540392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>430</v>
       </c>
       <c r="B21">
@@ -658,10 +2832,18 @@
       <c r="C21">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="1"/>
+        <v>0.25118864315095801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>435</v>
       </c>
       <c r="B22">
@@ -670,10 +2852,18 @@
       <c r="C22">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="1"/>
+        <v>0.28840315031266056</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>440</v>
       </c>
       <c r="B23">
@@ -682,10 +2872,18 @@
       <c r="C23">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30902954325135895</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>445</v>
       </c>
       <c r="B24">
@@ -694,10 +2892,18 @@
       <c r="C24">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31622776601683794</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>450</v>
       </c>
       <c r="B25">
@@ -706,10 +2912,18 @@
       <c r="C25">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30902954325135895</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="B26">
@@ -718,10 +2932,18 @@
       <c r="C26">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30199517204020154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>460</v>
       </c>
       <c r="B27">
@@ -730,10 +2952,18 @@
       <c r="C27">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30199517204020154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>465</v>
       </c>
       <c r="B28">
@@ -742,10 +2972,18 @@
       <c r="C28">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31622776601683794</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>470</v>
       </c>
       <c r="B29">
@@ -754,10 +2992,18 @@
       <c r="C29">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="1"/>
+        <v>0.32359365692962827</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>475</v>
       </c>
       <c r="B30">
@@ -766,10 +3012,18 @@
       <c r="C30">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31622776601683794</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>480</v>
       </c>
       <c r="B31">
@@ -778,10 +3032,18 @@
       <c r="C31">
         <v>53</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="1"/>
+        <v>0.29512092266663847</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>485</v>
       </c>
       <c r="B32">
@@ -790,10 +3052,18 @@
       <c r="C32">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="1"/>
+        <v>0.25703957827688634</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>490</v>
       </c>
       <c r="B33">
@@ -802,10 +3072,18 @@
       <c r="C33">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="1"/>
+        <v>0.22908676527677729</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>495</v>
       </c>
       <c r="B34">
@@ -814,10 +3092,18 @@
       <c r="C34">
         <v>64</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="1"/>
+        <v>0.22908676527677729</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>500</v>
       </c>
       <c r="B35">
@@ -826,10 +3112,18 @@
       <c r="C35">
         <v>62</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="1"/>
+        <v>0.23988329190194901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>505</v>
       </c>
       <c r="B36">
@@ -838,10 +3132,18 @@
       <c r="C36">
         <v>56</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="1"/>
+        <v>0.27542287033381663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>510</v>
       </c>
       <c r="B37">
@@ -850,8 +3152,16 @@
       <c r="C37">
         <v>51</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30902954325135895</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>515</v>
       </c>
@@ -861,8 +3171,16 @@
       <c r="C38">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" si="1"/>
+        <v>0.34673685045253166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>520</v>
       </c>
@@ -872,8 +3190,16 @@
       <c r="C39">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" si="1"/>
+        <v>0.3981071705534972</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>525</v>
       </c>
@@ -883,8 +3209,16 @@
       <c r="C40">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" si="1"/>
+        <v>0.41686938347033536</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>530</v>
       </c>
@@ -894,8 +3228,16 @@
       <c r="C41">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>0.41</v>
+      </c>
+      <c r="E41" s="4">
+        <f t="shared" si="1"/>
+        <v>0.38904514499428056</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>535</v>
       </c>
@@ -905,8 +3247,16 @@
       <c r="C42">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="E42" s="4">
+        <f t="shared" si="1"/>
+        <v>0.33113112148259105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>540</v>
       </c>
@@ -916,8 +3266,16 @@
       <c r="C43">
         <v>55</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E43" s="4">
+        <f t="shared" si="1"/>
+        <v>0.28183829312644532</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>545</v>
       </c>
@@ -927,8 +3285,16 @@
       <c r="C44">
         <v>66</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>0.66</v>
+      </c>
+      <c r="E44" s="4">
+        <f t="shared" si="1"/>
+        <v>0.21877616239495523</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>550</v>
       </c>
@@ -938,8 +3304,16 @@
       <c r="C45">
         <v>71</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19498445997580449</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>555</v>
       </c>
@@ -949,8 +3323,16 @@
       <c r="C46">
         <v>70</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="E46" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19952623149688795</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>560</v>
       </c>
@@ -960,8 +3342,16 @@
       <c r="C47">
         <v>64</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="E47" s="4">
+        <f t="shared" si="1"/>
+        <v>0.22908676527677729</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>565</v>
       </c>
@@ -971,8 +3361,16 @@
       <c r="C48">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E48" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31622776601683794</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>570</v>
       </c>
@@ -982,8 +3380,16 @@
       <c r="C49">
         <v>32</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="E49" s="4">
+        <f t="shared" si="1"/>
+        <v>0.47863009232263831</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>575</v>
       </c>
@@ -993,8 +3399,16 @@
       <c r="C50">
         <v>21</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>0.21</v>
+      </c>
+      <c r="E50" s="4">
+        <f t="shared" si="1"/>
+        <v>0.61659500186148219</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>580</v>
       </c>
@@ -1004,8 +3418,16 @@
       <c r="C51">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="E51" s="4">
+        <f t="shared" si="1"/>
+        <v>0.75857757502918366</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>585</v>
       </c>
@@ -1015,8 +3437,16 @@
       <c r="C52">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="E52" s="4">
+        <f t="shared" si="1"/>
+        <v>0.81283051616409918</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>590</v>
       </c>
@@ -1026,8 +3456,16 @@
       <c r="C53">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="E53" s="4">
+        <f t="shared" si="1"/>
+        <v>0.81283051616409918</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>595</v>
       </c>
@@ -1037,8 +3475,16 @@
       <c r="C54">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>0.13</v>
+      </c>
+      <c r="E54" s="4">
+        <f t="shared" si="1"/>
+        <v>0.74131024130091738</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>600</v>
       </c>
@@ -1048,8 +3494,16 @@
       <c r="C55">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+      <c r="E55" s="4">
+        <f t="shared" si="1"/>
+        <v>0.60255958607435778</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>605</v>
       </c>
@@ -1059,8 +3513,16 @@
       <c r="C56">
         <v>32</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="E56" s="4">
+        <f t="shared" si="1"/>
+        <v>0.47863009232263831</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>610</v>
       </c>
@@ -1070,8 +3532,16 @@
       <c r="C57">
         <v>42</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+      <c r="E57" s="4">
+        <f t="shared" si="1"/>
+        <v>0.38018939632056115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>615</v>
       </c>
@@ -1081,8 +3551,16 @@
       <c r="C58">
         <v>54</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+      <c r="E58" s="4">
+        <f t="shared" si="1"/>
+        <v>0.28840315031266056</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>620</v>
       </c>
@@ -1092,8 +3570,16 @@
       <c r="C59">
         <v>63</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>0.63</v>
+      </c>
+      <c r="E59" s="4">
+        <f t="shared" si="1"/>
+        <v>0.23442288153199217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>625</v>
       </c>
@@ -1103,8 +3589,16 @@
       <c r="C60">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>0.69</v>
+      </c>
+      <c r="E60" s="4">
+        <f t="shared" si="1"/>
+        <v>0.20417379446695291</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>630</v>
       </c>
@@ -1114,8 +3608,16 @@
       <c r="C61">
         <v>71</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="E61" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19498445997580449</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>635</v>
       </c>
@@ -1125,8 +3627,16 @@
       <c r="C62">
         <v>72</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+      <c r="E62" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19054607179632471</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>640</v>
       </c>
@@ -1136,8 +3646,16 @@
       <c r="C63">
         <v>71</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="E63" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19498445997580449</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>645</v>
       </c>
@@ -1147,8 +3665,16 @@
       <c r="C64">
         <v>71</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="E64" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19498445997580449</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>650</v>
       </c>
@@ -1158,8 +3684,16 @@
       <c r="C65">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="E65" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19952623149688795</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>655</v>
       </c>
@@ -1169,8 +3703,16 @@
       <c r="C66">
         <v>67</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>0.67</v>
+      </c>
+      <c r="E66" s="4">
+        <f t="shared" si="1"/>
+        <v>0.21379620895022314</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>660</v>
       </c>
@@ -1180,8 +3722,16 @@
       <c r="C67">
         <v>64</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <f t="shared" ref="D67:D111" si="3">C67/100</f>
+        <v>0.64</v>
+      </c>
+      <c r="E67" s="4">
+        <f t="shared" ref="E67:E111" si="4">10^(-C67/100)</f>
+        <v>0.22908676527677729</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>665</v>
       </c>
@@ -1191,8 +3741,16 @@
       <c r="C68">
         <v>62</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <f t="shared" si="3"/>
+        <v>0.62</v>
+      </c>
+      <c r="E68" s="4">
+        <f t="shared" si="4"/>
+        <v>0.23988329190194901</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>670</v>
       </c>
@@ -1202,8 +3760,16 @@
       <c r="C69">
         <v>58</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <f t="shared" si="3"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E69" s="4">
+        <f t="shared" si="4"/>
+        <v>0.2630267991895382</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>675</v>
       </c>
@@ -1213,8 +3779,16 @@
       <c r="C70">
         <v>54</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <f t="shared" si="3"/>
+        <v>0.54</v>
+      </c>
+      <c r="E70" s="4">
+        <f t="shared" si="4"/>
+        <v>0.28840315031266056</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>680</v>
       </c>
@@ -1224,8 +3798,16 @@
       <c r="C71">
         <v>49</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <f t="shared" si="3"/>
+        <v>0.49</v>
+      </c>
+      <c r="E71" s="4">
+        <f t="shared" si="4"/>
+        <v>0.32359365692962827</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>685</v>
       </c>
@@ -1235,8 +3817,16 @@
       <c r="C72">
         <v>44</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <f t="shared" si="3"/>
+        <v>0.44</v>
+      </c>
+      <c r="E72" s="4">
+        <f t="shared" si="4"/>
+        <v>0.36307805477010135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>690</v>
       </c>
@@ -1246,8 +3836,16 @@
       <c r="C73">
         <v>43</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <f t="shared" si="3"/>
+        <v>0.43</v>
+      </c>
+      <c r="E73" s="4">
+        <f t="shared" si="4"/>
+        <v>0.37153522909717251</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>695</v>
       </c>
@@ -1257,8 +3855,16 @@
       <c r="C74">
         <v>40</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="E74" s="4">
+        <f t="shared" si="4"/>
+        <v>0.3981071705534972</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>700</v>
       </c>
@@ -1268,8 +3874,16 @@
       <c r="C75">
         <v>38</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <f t="shared" si="3"/>
+        <v>0.38</v>
+      </c>
+      <c r="E75" s="4">
+        <f t="shared" si="4"/>
+        <v>0.41686938347033536</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>705</v>
       </c>
@@ -1279,8 +3893,16 @@
       <c r="C76">
         <v>35</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <f t="shared" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="E76" s="4">
+        <f t="shared" si="4"/>
+        <v>0.44668359215096315</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>710</v>
       </c>
@@ -1290,8 +3912,16 @@
       <c r="C77">
         <v>35</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <f t="shared" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="E77" s="4">
+        <f t="shared" si="4"/>
+        <v>0.44668359215096315</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>715</v>
       </c>
@@ -1301,8 +3931,16 @@
       <c r="C78">
         <v>34</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <f t="shared" si="3"/>
+        <v>0.34</v>
+      </c>
+      <c r="E78" s="4">
+        <f t="shared" si="4"/>
+        <v>0.45708818961487502</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>720</v>
       </c>
@@ -1312,8 +3950,16 @@
       <c r="C79">
         <v>35</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <f t="shared" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="E79" s="4">
+        <f t="shared" si="4"/>
+        <v>0.44668359215096315</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>725</v>
       </c>
@@ -1323,8 +3969,16 @@
       <c r="C80">
         <v>39</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <f t="shared" si="3"/>
+        <v>0.39</v>
+      </c>
+      <c r="E80" s="4">
+        <f t="shared" si="4"/>
+        <v>0.40738027780411268</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>730</v>
       </c>
@@ -1334,8 +3988,16 @@
       <c r="C81">
         <v>41</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <f t="shared" si="3"/>
+        <v>0.41</v>
+      </c>
+      <c r="E81" s="4">
+        <f t="shared" si="4"/>
+        <v>0.38904514499428056</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>735</v>
       </c>
@@ -1345,8 +4007,16 @@
       <c r="C82">
         <v>46</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <f t="shared" si="3"/>
+        <v>0.46</v>
+      </c>
+      <c r="E82" s="4">
+        <f t="shared" si="4"/>
+        <v>0.34673685045253166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>740</v>
       </c>
@@ -1356,8 +4026,16 @@
       <c r="C83">
         <v>49</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <f t="shared" si="3"/>
+        <v>0.49</v>
+      </c>
+      <c r="E83" s="4">
+        <f t="shared" si="4"/>
+        <v>0.32359365692962827</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>745</v>
       </c>
@@ -1367,8 +4045,16 @@
       <c r="C84">
         <v>51</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+      <c r="E84" s="4">
+        <f t="shared" si="4"/>
+        <v>0.30902954325135895</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>750</v>
       </c>
@@ -1378,8 +4064,16 @@
       <c r="C85">
         <v>54</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <f t="shared" si="3"/>
+        <v>0.54</v>
+      </c>
+      <c r="E85" s="4">
+        <f t="shared" si="4"/>
+        <v>0.28840315031266056</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>755</v>
       </c>
@@ -1389,8 +4083,16 @@
       <c r="C86">
         <v>58</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <f t="shared" si="3"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E86" s="4">
+        <f t="shared" si="4"/>
+        <v>0.2630267991895382</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>760</v>
       </c>
@@ -1400,8 +4102,16 @@
       <c r="C87">
         <v>60</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="E87" s="4">
+        <f t="shared" si="4"/>
+        <v>0.25118864315095801</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>765</v>
       </c>
@@ -1411,8 +4121,16 @@
       <c r="C88">
         <v>62</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <f t="shared" si="3"/>
+        <v>0.62</v>
+      </c>
+      <c r="E88" s="4">
+        <f t="shared" si="4"/>
+        <v>0.23988329190194901</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>770</v>
       </c>
@@ -1422,8 +4140,16 @@
       <c r="C89">
         <v>64</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <f t="shared" si="3"/>
+        <v>0.64</v>
+      </c>
+      <c r="E89" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22908676527677729</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>775</v>
       </c>
@@ -1433,8 +4159,16 @@
       <c r="C90">
         <v>67</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <f t="shared" si="3"/>
+        <v>0.67</v>
+      </c>
+      <c r="E90" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21379620895022314</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>780</v>
       </c>
@@ -1444,8 +4178,16 @@
       <c r="C91">
         <v>67</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <f t="shared" si="3"/>
+        <v>0.67</v>
+      </c>
+      <c r="E91" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21379620895022314</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>785</v>
       </c>
@@ -1455,8 +4197,16 @@
       <c r="C92">
         <v>69</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <f t="shared" si="3"/>
+        <v>0.69</v>
+      </c>
+      <c r="E92" s="4">
+        <f t="shared" si="4"/>
+        <v>0.20417379446695291</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>790</v>
       </c>
@@ -1466,8 +4216,16 @@
       <c r="C93">
         <v>69</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <f t="shared" si="3"/>
+        <v>0.69</v>
+      </c>
+      <c r="E93" s="4">
+        <f t="shared" si="4"/>
+        <v>0.20417379446695291</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>795</v>
       </c>
@@ -1477,8 +4235,16 @@
       <c r="C94">
         <v>70</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="E94" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19952623149688795</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>800</v>
       </c>
@@ -1488,8 +4254,16 @@
       <c r="C95">
         <v>71</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <f t="shared" si="3"/>
+        <v>0.71</v>
+      </c>
+      <c r="E95" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19498445997580449</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>805</v>
       </c>
@@ -1499,8 +4273,16 @@
       <c r="C96">
         <v>72</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <f t="shared" si="3"/>
+        <v>0.72</v>
+      </c>
+      <c r="E96" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19054607179632471</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <f>A96+5</f>
         <v>810</v>
@@ -1511,10 +4293,18 @@
       <c r="C97">
         <v>73</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <f t="shared" si="3"/>
+        <v>0.73</v>
+      </c>
+      <c r="E97" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18620871366628672</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <f t="shared" ref="A98:A125" si="1">A97+5</f>
+        <f t="shared" ref="A98:A125" si="5">A97+5</f>
         <v>815</v>
       </c>
       <c r="B98">
@@ -1523,10 +4313,18 @@
       <c r="C98">
         <v>74</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <f t="shared" si="3"/>
+        <v>0.74</v>
+      </c>
+      <c r="E98" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18197008586099833</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>820</v>
       </c>
       <c r="B99">
@@ -1535,10 +4333,18 @@
       <c r="C99">
         <v>74</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <f t="shared" si="3"/>
+        <v>0.74</v>
+      </c>
+      <c r="E99" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18197008586099833</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>825</v>
       </c>
       <c r="B100">
@@ -1547,10 +4353,18 @@
       <c r="C100">
         <v>75</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="E100" s="4">
+        <f t="shared" si="4"/>
+        <v>0.17782794100389224</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>830</v>
       </c>
       <c r="B101">
@@ -1559,10 +4373,18 @@
       <c r="C101">
         <v>75</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="E101" s="4">
+        <f t="shared" si="4"/>
+        <v>0.17782794100389224</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>835</v>
       </c>
       <c r="B102">
@@ -1571,10 +4393,18 @@
       <c r="C102">
         <v>75</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="E102" s="4">
+        <f t="shared" si="4"/>
+        <v>0.17782794100389224</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>840</v>
       </c>
       <c r="B103">
@@ -1583,10 +4413,18 @@
       <c r="C103">
         <v>74</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <f t="shared" si="3"/>
+        <v>0.74</v>
+      </c>
+      <c r="E103" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18197008586099833</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>845</v>
       </c>
       <c r="B104">
@@ -1595,10 +4433,18 @@
       <c r="C104">
         <v>72</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <f t="shared" si="3"/>
+        <v>0.72</v>
+      </c>
+      <c r="E104" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19054607179632471</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>850</v>
       </c>
       <c r="B105">
@@ -1607,10 +4453,18 @@
       <c r="C105">
         <v>69</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <f t="shared" si="3"/>
+        <v>0.69</v>
+      </c>
+      <c r="E105" s="4">
+        <f t="shared" si="4"/>
+        <v>0.20417379446695291</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>855</v>
       </c>
       <c r="B106">
@@ -1619,10 +4473,18 @@
       <c r="C106">
         <v>64</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <f t="shared" si="3"/>
+        <v>0.64</v>
+      </c>
+      <c r="E106" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22908676527677729</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>860</v>
       </c>
       <c r="B107">
@@ -1631,10 +4493,18 @@
       <c r="C107">
         <v>59</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <f t="shared" si="3"/>
+        <v>0.59</v>
+      </c>
+      <c r="E107" s="4">
+        <f t="shared" si="4"/>
+        <v>0.25703957827688634</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>865</v>
       </c>
       <c r="B108">
@@ -1643,10 +4513,18 @@
       <c r="C108">
         <v>54</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <f t="shared" si="3"/>
+        <v>0.54</v>
+      </c>
+      <c r="E108" s="4">
+        <f t="shared" si="4"/>
+        <v>0.28840315031266056</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>870</v>
       </c>
       <c r="B109">
@@ -1655,10 +4533,18 @@
       <c r="C109">
         <v>50</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="E109" s="4">
+        <f t="shared" si="4"/>
+        <v>0.31622776601683794</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>875</v>
       </c>
       <c r="B110">
@@ -1667,10 +4553,18 @@
       <c r="C110">
         <v>48</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <f t="shared" si="3"/>
+        <v>0.48</v>
+      </c>
+      <c r="E110" s="4">
+        <f t="shared" si="4"/>
+        <v>0.33113112148259105</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>880</v>
       </c>
       <c r="B111">
@@ -1679,92 +4573,101 @@
       <c r="C111">
         <v>46</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <f t="shared" si="3"/>
+        <v>0.46</v>
+      </c>
+      <c r="E111" s="4">
+        <f t="shared" si="4"/>
+        <v>0.34673685045253166</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>885</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>890</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>895</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>905</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>910</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>915</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>920</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>925</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>930</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>935</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>940</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>945</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>950</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>